<commit_message>
ALS and ESRD items added
ALS and ESRD definitions, flags and indicators added to data dictionary
</commit_message>
<xml_diff>
--- a/Data_dictionary.xlsx
+++ b/Data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Bell\_BIP\Consults\Walling - Bell\Sent to Other Sites 08302018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsanz\Documents\GitHub\UC_Event_Care_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>SAMPLE GROUP</t>
   </si>
@@ -266,21 +266,53 @@
     <t>Instructions for the abstraction portion of the form</t>
   </si>
   <si>
-    <t>This is whether the condition by which the patient was identified as having advanced illness is present as advanced illness in this patient.  Please use the following advanced illness definitions:
+    <t>Patient has a LVEF result &lt;= 31 in the last three years (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>"This is whether the condition by which the patient was identified as having advanced illness is present as advanced illness in this patient.  Please use the following advanced illness definitions:
 * Advanced cancer – Solid tumor or hematologic cancer that is incurable
 * Advanced heart failure – Diagnosed heart failure AND heart failure substantially affects the patient’s function {[(shortness of breath or weakness or chest pain or ectopy with exertion or edema affecting function or cannot do activities) and not due to another cause] or class 3 or 4} OR last known LVEF &lt; 31%
 * Advanced COPD - Diagnosed COPD AND COPD substantially affects the patient’s function [(shortness of breath with exertion or cannot do activities and not due to another cause) or GOLD class 3 or 4] OR (PFTs show FEV1/FVC &lt;0.70 and FEV1 &lt;50% predicted) OR O2-dependent at home (all the time or for exertion but not just at night)
-* Decompensated cirrhosis - Cirrhosis with evidence of decompensation represented by ascites, esophageal variceal bleeding, hepatorenal syndrome or hepatic encephalopathy.</t>
-  </si>
-  <si>
-    <t>Patient has a LVEF result &lt;= 31 in the last three years (1 = yes, 0 = no)</t>
+* Decompensated cirrhosis - Cirrhosis with evidence of decompensation represented by ascites, esophageal variceal bleeding, hepatorenal syndrome or hepatic encephalopathy."
+* ALS with progressive symptoms impacting functional status
+* ESRD:  CKD  on HD or HD/renal transplant being actively considered or H/0 renal transplant</t>
+  </si>
+  <si>
+    <t>PL_ALS</t>
+  </si>
+  <si>
+    <t>ALS diagnoses found in PL (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>PL_ESRD</t>
+  </si>
+  <si>
+    <t>ESRD diagnoses found in PL (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>DX_ALD</t>
+  </si>
+  <si>
+    <t>ALS diagnoses found in encounter dx (Office Visit) (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>DX_ESRD</t>
+  </si>
+  <si>
+    <t>ESRD diagnoses found in encounter dx (Office Visit) (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>NEPH_VISIT</t>
+  </si>
+  <si>
+    <t>Indicates if the patient had an nephrology encounter in the last 12 months (1 = yes, 0 = no)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +335,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -390,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -414,6 +452,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,7 +488,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -491,13 +535,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>371476</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -806,11 +850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +864,7 @@
     <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -828,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -836,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -844,7 +888,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -852,306 +896,354 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="D8" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="9"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B41" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>